<commit_message>
Design file up to winding selection (wire diameter etc.)
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Designfile.xlsx
+++ b/Project/BAP/Design/Designfile.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="3" r:id="rId2"/>
-    <sheet name="Burdadursun" sheetId="2" r:id="rId3"/>
+    <sheet name="General Calculations" sheetId="4" r:id="rId2"/>
+    <sheet name="Drive Calculations" sheetId="5" r:id="rId3"/>
+    <sheet name="Calculations" sheetId="3" r:id="rId4"/>
+    <sheet name="Burdadursun" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="108">
   <si>
     <t>Power factor</t>
   </si>
@@ -38,39 +40,6 @@
   </si>
   <si>
     <t>Number of poles</t>
-  </si>
-  <si>
-    <t>Teeth flux density</t>
-  </si>
-  <si>
-    <t>&lt;1.7</t>
-  </si>
-  <si>
-    <t>Outer diameter (mm)</t>
-  </si>
-  <si>
-    <t>Cogging torque (%)</t>
-  </si>
-  <si>
-    <t>&lt;2</t>
-  </si>
-  <si>
-    <t>Inner diameter (mm)</t>
-  </si>
-  <si>
-    <t>Axial length (mm)</t>
-  </si>
-  <si>
-    <t>Magnet length (mm)</t>
-  </si>
-  <si>
-    <t>Gap distance (mm)</t>
-  </si>
-  <si>
-    <t>Shaft diameter</t>
-  </si>
-  <si>
-    <t>Number of turns per coil side</t>
   </si>
   <si>
     <t>Symbol</t>
@@ -700,9 +669,6 @@
     </r>
   </si>
   <si>
-    <t>not designed</t>
-  </si>
-  <si>
     <t>play with this</t>
   </si>
   <si>
@@ -725,15 +691,129 @@
     </r>
   </si>
   <si>
-    <t>Next is the induced voltage</t>
+    <t>pole</t>
+  </si>
+  <si>
+    <t>Do/Di</t>
+  </si>
+  <si>
+    <t>Stator slot pitch</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Flux per pole</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>pp</t>
+    </r>
+  </si>
+  <si>
+    <t>mWb</t>
+  </si>
+  <si>
+    <t>Turns per coil side</t>
+  </si>
+  <si>
+    <t>Layer number</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <r>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+  </si>
+  <si>
+    <t>Induced voltage (module-phase)</t>
+  </si>
+  <si>
+    <r>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>Turns per module per phase</t>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -783,7 +863,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,8 +876,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -820,22 +906,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -852,25 +927,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1155,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,248 +1263,279 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7">
         <v>8000</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G2" s="7">
         <v>94</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>540</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G3" s="7">
         <v>0.9</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G4" s="7">
         <v>98</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C5" s="7">
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C6" s="7">
         <v>0.85</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C8" s="7">
         <v>600</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="10">
+        <v>62</v>
+      </c>
+      <c r="G8" s="9">
         <v>3.1415926500000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C10" s="7">
         <v>0.6</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7">
         <v>50</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C12" s="7">
         <v>0.9</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7">
         <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
@@ -1434,350 +1550,1624 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7">
         <f>Parameters!C4/Parameters!C5</f>
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7">
         <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
         <v>24</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C4" s="7">
         <f>Parameters!C9*10</f>
         <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C5" s="7">
         <f>C3/(C4*Parameters!C7)</f>
         <v>0.4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="13">
+        <v>2</v>
+      </c>
+      <c r="I5" s="13">
+        <v>4</v>
+      </c>
+      <c r="J5" s="13">
+        <v>6</v>
+      </c>
+      <c r="K5" s="13">
+        <v>8</v>
+      </c>
+      <c r="L5" s="13">
+        <v>10</v>
+      </c>
+      <c r="M5" s="13">
+        <v>12</v>
+      </c>
+      <c r="N5" s="13">
+        <v>14</v>
+      </c>
+      <c r="O5" s="13">
+        <v>16</v>
+      </c>
+      <c r="P5" s="13">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7">
         <v>0.93300000000000005</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="9">
-        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
-        <v>127.32395461900511</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.88</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1.78</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1.66</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1.54</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1.43</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="G7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="15">
+        <f>2-((H5)/2-1)*0.1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="15">
+        <f>2-((I5)/2-1)*0.115</f>
+        <v>1.885</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
+        <v>1.77</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.655</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="N7" s="15">
+        <f>2-((N5)/2-1)*0.11</f>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
+        <v>1.23</v>
+      </c>
+      <c r="P7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+      <c r="R7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="9">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8">
         <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
         <v>2127.6595744680853</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C9" s="7">
         <f>Parameters!C3/Parameters!C5</f>
         <v>270</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="9">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8">
         <f>0.612*Parameters!C6*C9/SQRT(3)</f>
         <v>81.091154708759703</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="9">
-        <f>C8/(Parameters!G3*Calculations!C10*3)</f>
+        <v>69</v>
+      </c>
+      <c r="C11" s="8">
+        <f>C8/(Parameters!G3*'General Calculations'!C10*3)</f>
         <v>9.7177314523144265</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C12" s="7">
-        <f>Parameters!C8*Calculations!C4/120</f>
+        <f>Parameters!C8*'General Calculations'!C4/120</f>
         <v>100</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C13" s="7">
         <f>Parameters!C11*Parameters!C12</f>
         <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="12">
+        <v>75</v>
+      </c>
+      <c r="C14" s="10">
         <f>2*C7/(C13*1000*Parameters!G8)</f>
-        <v>1.8012654910913857E-3</v>
+        <v>0</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="J14">
+        <f>0.155^2*150</f>
+        <v>3.6037500000000002</v>
+      </c>
+      <c r="K14">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="13">
+        <v>80</v>
+      </c>
+      <c r="C16" s="11">
         <f>1000*(C14/C15)^(1/3)</f>
-        <v>208.05711769225979</v>
+        <v>0</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="11">
+        <f>C16*C15</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="11">
+        <f>C18*C16</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="7">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="13">
-        <f>C16*C15</f>
-        <v>41.611423538451959</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="B21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="8">
+        <f>Parameters!G8*'General Calculations'!C16/'General Calculations'!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="13">
-        <f>1.2*C16</f>
-        <v>249.66854123071175</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="14" t="s">
+      <c r="B22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="16">
+        <f>0.001*2*C16*C17*Parameters!C12/'General Calculations'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="7">
-        <v>3</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C23" s="7">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="7">
+        <f>C23*Parameters!C9*Parameters!C15/2</f>
+        <v>200</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D30" s="3"/>
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="8">
+        <f>4.44*C24*C12*C22*C6/1000</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R36"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7">
+        <f>Parameters!C4/Parameters!C5</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Parameters!C9*10</f>
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C3/(C4*Parameters!C7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="13">
+        <v>2</v>
+      </c>
+      <c r="I5" s="13">
+        <v>4</v>
+      </c>
+      <c r="J5" s="13">
+        <v>6</v>
+      </c>
+      <c r="K5" s="13">
+        <v>8</v>
+      </c>
+      <c r="L5" s="13">
+        <v>10</v>
+      </c>
+      <c r="M5" s="13">
+        <v>12</v>
+      </c>
+      <c r="N5" s="13">
+        <v>14</v>
+      </c>
+      <c r="O5" s="13">
+        <v>16</v>
+      </c>
+      <c r="P5" s="13">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.88</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1.78</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1.66</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1.54</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1.43</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8">
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
+        <v>127.32395461900511</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="15">
+        <f>2-((H5)/2-1)*0.1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="15">
+        <f>2-((I5)/2-1)*0.115</f>
+        <v>1.885</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
+        <v>1.77</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.655</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="N7" s="15">
+        <f>2-((N5)/2-1)*0.11</f>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
+        <v>1.23</v>
+      </c>
+      <c r="P7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+      <c r="R7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8">
+        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
+        <v>2127.6595744680853</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="7">
+        <f>Parameters!C3/Parameters!C5</f>
+        <v>270</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8">
+        <f>0.612*Parameters!C6*C9/SQRT(3)</f>
+        <v>81.091154708759703</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="8">
+        <f>C8/(Parameters!G3*'Drive Calculations'!C10*3)</f>
+        <v>9.7177314523144265</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7">
+        <f>Parameters!C8*'Drive Calculations'!C4/120</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="7">
+        <f>Parameters!C11*Parameters!C12</f>
+        <v>45</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="10">
+        <f>2*C7/(C13*1000*Parameters!G8)</f>
+        <v>1.8012654910913857E-3</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14">
+        <f>0.155^2*150</f>
+        <v>3.6037500000000002</v>
+      </c>
+      <c r="K14">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="11">
+        <f>1000*(C14/C15)^(1/3)</f>
+        <v>181.7546335652992</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="11">
+        <f>C16*C15</f>
+        <v>54.526390069589759</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="11">
+        <f>C18*C16</f>
+        <v>254.45648699141887</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="7">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="8">
+        <f>Parameters!G8*'Drive Calculations'!C16/'Drive Calculations'!C3</f>
+        <v>23.791625871341139</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="16">
+        <f>0.001*2*C16*C17*Parameters!C12/'Drive Calculations'!C4</f>
+        <v>0.891938164206317</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="7">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="7">
+        <f>C23*Parameters!C9*Parameters!C15/2</f>
+        <v>200</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="8">
+        <f>4.44*C24*C12*C22*C6/1000</f>
+        <v>73.897433679759047</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R36"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7">
+        <f>Parameters!C4/Parameters!C5</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Parameters!C9*10</f>
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C3/(C4*Parameters!C7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="13">
+        <v>2</v>
+      </c>
+      <c r="I5" s="13">
+        <v>4</v>
+      </c>
+      <c r="J5" s="13">
+        <v>6</v>
+      </c>
+      <c r="K5" s="13">
+        <v>8</v>
+      </c>
+      <c r="L5" s="13">
+        <v>10</v>
+      </c>
+      <c r="M5" s="13">
+        <v>12</v>
+      </c>
+      <c r="N5" s="13">
+        <v>14</v>
+      </c>
+      <c r="O5" s="13">
+        <v>16</v>
+      </c>
+      <c r="P5" s="13">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.88</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1.78</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1.66</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1.54</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1.43</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8">
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
+        <v>127.32395461900511</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="15">
+        <f>2-((H5)/2-1)*0.1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="15">
+        <f>2-((I5)/2-1)*0.115</f>
+        <v>1.885</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
+        <v>1.77</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.655</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="N7" s="15">
+        <f>2-((N5)/2-1)*0.11</f>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
+        <v>1.23</v>
+      </c>
+      <c r="P7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+      <c r="R7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8">
+        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
+        <v>2127.6595744680853</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="7">
+        <f>Parameters!C3/Parameters!C5</f>
+        <v>270</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8">
+        <f>0.612*Parameters!C6*C9/SQRT(3)</f>
+        <v>81.091154708759703</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="8">
+        <f>C8/(Parameters!G3*Calculations!C10*3)</f>
+        <v>9.7177314523144265</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7">
+        <f>Parameters!C8*Calculations!C4/120</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="7">
+        <f>Parameters!C11*Parameters!C12</f>
+        <v>45</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="10">
+        <f>2*C7/(C13*1000*Parameters!G8)</f>
+        <v>1.8012654910913857E-3</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14">
+        <f>0.155^2*150</f>
+        <v>3.6037500000000002</v>
+      </c>
+      <c r="K14">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="11">
+        <f>1000*(C14/C15)^(1/3)</f>
+        <v>181.7546335652992</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="11">
+        <f>C16*C15</f>
+        <v>54.526390069589759</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="11">
+        <f>C18*C16</f>
+        <v>254.45648699141887</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="7">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="8">
+        <f>Parameters!G8*Calculations!C16/Calculations!C3</f>
+        <v>23.791625871341139</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="16">
+        <f>0.001*2*C16*C17*Parameters!C12/Calculations!C4</f>
+        <v>0.891938164206317</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="7">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="7">
+        <f>C23*Parameters!C9*Parameters!C15/2</f>
+        <v>200</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="8">
+        <f>4.44*C24*C12*C22*C6/1000</f>
+        <v>73.897433679759047</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C19" sqref="A1:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,65 +3176,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="2">
-        <v>220</v>
-      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2">
-        <v>155</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2">
-        <v>150</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="2">
-        <v>75</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>35</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -1887,21 +3251,13 @@
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Design on excel up to slot fill factor. Fill factor is currently 1.6, which is not possible. Maxwell says it is 0.6.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Designfile.xlsx
+++ b/Project/BAP/Design/Designfile.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="General Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="Drive Calculations" sheetId="5" r:id="rId3"/>
-    <sheet name="Calculations" sheetId="3" r:id="rId4"/>
-    <sheet name="Burdadursun" sheetId="2" r:id="rId5"/>
+    <sheet name="Calculations-old" sheetId="3" r:id="rId3"/>
+    <sheet name="Burdadursun" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
   <si>
     <t>Power factor</t>
   </si>
@@ -805,6 +804,84 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Inh</t>
+  </si>
+  <si>
+    <t>Copper resistivity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>Copper permeability</t>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>H/m</t>
+  </si>
+  <si>
+    <t>Skin depth</t>
+  </si>
+  <si>
+    <t>δ</t>
   </si>
 </sst>
 </file>
@@ -815,7 +892,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +939,22 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -883,7 +976,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -906,11 +999,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -928,9 +1071,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -956,6 +1096,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1240,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1426,7 @@
     <col min="4" max="4" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1411,6 +1585,12 @@
       <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E7" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
@@ -1427,17 +1607,18 @@
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>3.1415926500000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1449,6 +1630,18 @@
       </c>
       <c r="D9" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1.7E-8</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1464,6 +1657,18 @@
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="31">
+        <v>1.2566289999999999E-6</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
@@ -1478,6 +1683,10 @@
       <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -1492,6 +1701,10 @@
       <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1506,6 +1719,10 @@
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
@@ -1543,6 +1760,9 @@
       <c r="H30" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E7:H7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1550,10 +1770,570 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="7">
+        <f>Parameters!C4/Parameters!C5</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Parameters!C9*10</f>
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="10">
+        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
+        <v>2127.6595744680853</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C3/(C4*Parameters!C7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="7">
+        <f>Parameters!C3/Parameters!C5</f>
+        <v>270</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="8">
+        <f>0.612*Parameters!C6*H5/SQRT(3)</f>
+        <v>81.091154708759703</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="7">
+        <f>Parameters!C11*Parameters!C12</f>
+        <v>45</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="8">
+        <f>H4/(Parameters!G3*'General Calculations'!H6*3)</f>
+        <v>9.7177314523144265</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="8">
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
+        <v>127.32395461900511</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="7">
+        <f>Parameters!C8*'General Calculations'!C4/120</f>
+        <v>100</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="28"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="9">
+        <f>2*C8/(C7*1000*Parameters!G8)</f>
+        <v>1.8012654910913857E-3</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="20">
+        <f>1000*(C9/C10)^(1/3)</f>
+        <v>181.7546335652992</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="10">
+        <f>C11*C10</f>
+        <v>54.526390069589759</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="10">
+        <f>C13*C11</f>
+        <v>254.45648699141887</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="7">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="8">
+        <f>Parameters!G8*C11/'General Calculations'!C3</f>
+        <v>23.791625871341139</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="15">
+        <f>0.001*2*C11*C12*Parameters!C12/'General Calculations'!C4</f>
+        <v>0.891938164206317</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="7">
+        <v>100</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="7">
+        <f>C18*Parameters!C9*Parameters!C15/2</f>
+        <v>200</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="8">
+        <f>4.44*C19*H8*C17*C6/1000</f>
+        <v>73.897433679759047</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="8">
+        <f>1000*SQRT(2*Parameters!G9/(2*Parameters!G8*H8*Parameters!G10))</f>
+        <v>6.562147464226471</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,37 +2420,37 @@
       <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>2</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>4</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>6</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>8</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>10</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="12">
         <v>12</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <v>14</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>16</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="12">
         <v>18</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1687,80 +2467,89 @@
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>2</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>1.88</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <v>1.78</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <v>1.66</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="14">
         <v>1.54</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <v>1.43</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
-      <c r="G7" s="14" t="s">
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8">
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
+        <v>127.32395461900511</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f>2-((H5)/2-1)*0.1</f>
         <v>2</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <f>2-((I5)/2-1)*0.115</f>
         <v>1.885</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
         <v>1.77</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="14">
         <f t="shared" si="0"/>
         <v>1.655</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="14">
         <f t="shared" si="0"/>
         <v>1.54</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <f t="shared" si="0"/>
         <v>1.4249999999999998</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="14">
         <f>2-((N5)/2-1)*0.11</f>
         <v>1.3399999999999999</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="14">
         <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
         <v>1.23</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="14">
         <f t="shared" si="1"/>
         <v>1.1200000000000001</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="14">
         <f t="shared" si="1"/>
         <v>1.01</v>
       </c>
@@ -1821,7 +2610,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="8">
-        <f>C8/(Parameters!G3*'General Calculations'!C10*3)</f>
+        <f>C8/(Parameters!G3*'Calculations-old'!C10*3)</f>
         <v>9.7177314523144265</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1836,7 +2625,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="7">
-        <f>Parameters!C8*'General Calculations'!C4/120</f>
+        <f>Parameters!C8*'Calculations-old'!C4/120</f>
         <v>100</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1865,9 +2654,9 @@
       <c r="B14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f>2*C7/(C13*1000*Parameters!G8)</f>
-        <v>0</v>
+        <v>1.8012654910913857E-3</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>76</v>
@@ -1893,7 +2682,7 @@
       <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>88</v>
       </c>
       <c r="K15">
@@ -1907,9 +2696,9 @@
       <c r="B16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <f>1000*(C14/C15)^(1/3)</f>
-        <v>0</v>
+        <v>181.7546335652992</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>81</v>
@@ -1922,14 +2711,14 @@
       <c r="B17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <f>C16*C15</f>
-        <v>0</v>
+        <v>54.526390069589759</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -1944,7 +2733,7 @@
       <c r="D18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1955,9 +2744,9 @@
       <c r="B19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <f>C18*C16</f>
-        <v>0</v>
+        <v>254.45648699141887</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>81</v>
@@ -1977,7 +2766,7 @@
       <c r="D20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
@@ -1987,8 +2776,8 @@
         <v>96</v>
       </c>
       <c r="C21" s="8">
-        <f>Parameters!G8*'General Calculations'!C16/'General Calculations'!C3</f>
-        <v>0</v>
+        <f>Parameters!G8*'Calculations-old'!C16/'Calculations-old'!C3</f>
+        <v>23.791625871341139</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>81</v>
@@ -2001,549 +2790,8 @@
       <c r="B22" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="16">
-        <f>0.001*2*C16*C17*Parameters!C12/'General Calculations'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="7">
-        <v>100</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="7">
-        <f>C23*Parameters!C9*Parameters!C15/2</f>
-        <v>200</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="8">
-        <f>4.44*C24*C12*C22*C6/1000</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="7">
-        <f>Parameters!C4/Parameters!C5</f>
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="7">
-        <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7">
-        <f>Parameters!C9*10</f>
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="7">
-        <f>C3/(C4*Parameters!C7)</f>
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="13">
-        <v>2</v>
-      </c>
-      <c r="I5" s="13">
-        <v>4</v>
-      </c>
-      <c r="J5" s="13">
-        <v>6</v>
-      </c>
-      <c r="K5" s="13">
-        <v>8</v>
-      </c>
-      <c r="L5" s="13">
-        <v>10</v>
-      </c>
-      <c r="M5" s="13">
-        <v>12</v>
-      </c>
-      <c r="N5" s="13">
-        <v>14</v>
-      </c>
-      <c r="O5" s="13">
-        <v>16</v>
-      </c>
-      <c r="P5" s="13">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="15">
-        <v>2</v>
-      </c>
-      <c r="I6" s="15">
-        <v>1.88</v>
-      </c>
-      <c r="J6" s="15">
-        <v>1.78</v>
-      </c>
-      <c r="K6" s="15">
-        <v>1.66</v>
-      </c>
-      <c r="L6" s="15">
-        <v>1.54</v>
-      </c>
-      <c r="M6" s="15">
-        <v>1.43</v>
-      </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="8">
-        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
-        <v>127.32395461900511</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="15">
-        <f>2-((H5)/2-1)*0.1</f>
-        <v>2</v>
-      </c>
-      <c r="I7" s="15">
-        <f>2-((I5)/2-1)*0.115</f>
-        <v>1.885</v>
-      </c>
-      <c r="J7" s="15">
-        <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
-        <v>1.77</v>
-      </c>
-      <c r="K7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.655</v>
-      </c>
-      <c r="L7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-      <c r="M7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.4249999999999998</v>
-      </c>
-      <c r="N7" s="15">
-        <f>2-((N5)/2-1)*0.11</f>
-        <v>1.3399999999999999</v>
-      </c>
-      <c r="O7" s="15">
-        <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
-        <v>1.23</v>
-      </c>
-      <c r="P7" s="15">
-        <f t="shared" si="1"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q7" s="15">
-        <f t="shared" si="1"/>
-        <v>1.01</v>
-      </c>
-      <c r="R7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="8">
-        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
-        <v>2127.6595744680853</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="7">
-        <f>Parameters!C3/Parameters!C5</f>
-        <v>270</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="8">
-        <f>0.612*Parameters!C6*C9/SQRT(3)</f>
-        <v>81.091154708759703</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="8">
-        <f>C8/(Parameters!G3*'Drive Calculations'!C10*3)</f>
-        <v>9.7177314523144265</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="7">
-        <f>Parameters!C8*'Drive Calculations'!C4/120</f>
-        <v>100</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="7">
-        <f>Parameters!C11*Parameters!C12</f>
-        <v>45</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="10">
-        <f>2*C7/(C13*1000*Parameters!G8)</f>
-        <v>1.8012654910913857E-3</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14">
-        <f>0.155^2*150</f>
-        <v>3.6037500000000002</v>
-      </c>
-      <c r="K14">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="11">
-        <f>1000*(C14/C15)^(1/3)</f>
-        <v>181.7546335652992</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="11">
-        <f>C16*C15</f>
-        <v>54.526390069589759</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="11">
-        <f>C18*C16</f>
-        <v>254.45648699141887</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="7">
-        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="8">
-        <f>Parameters!G8*'Drive Calculations'!C16/'Drive Calculations'!C3</f>
-        <v>23.791625871341139</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="16">
-        <f>0.001*2*C16*C17*Parameters!C12/'Drive Calculations'!C4</f>
+      <c r="C22" s="15">
+        <f>0.001*2*C16*C17*Parameters!C12/'Calculations-old'!C4</f>
         <v>0.891938164206317</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -2623,551 +2871,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="7">
-        <f>Parameters!C4/Parameters!C5</f>
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="7">
-        <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7">
-        <f>Parameters!C9*10</f>
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="7">
-        <f>C3/(C4*Parameters!C7)</f>
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="13">
-        <v>2</v>
-      </c>
-      <c r="I5" s="13">
-        <v>4</v>
-      </c>
-      <c r="J5" s="13">
-        <v>6</v>
-      </c>
-      <c r="K5" s="13">
-        <v>8</v>
-      </c>
-      <c r="L5" s="13">
-        <v>10</v>
-      </c>
-      <c r="M5" s="13">
-        <v>12</v>
-      </c>
-      <c r="N5" s="13">
-        <v>14</v>
-      </c>
-      <c r="O5" s="13">
-        <v>16</v>
-      </c>
-      <c r="P5" s="13">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="15">
-        <v>2</v>
-      </c>
-      <c r="I6" s="15">
-        <v>1.88</v>
-      </c>
-      <c r="J6" s="15">
-        <v>1.78</v>
-      </c>
-      <c r="K6" s="15">
-        <v>1.66</v>
-      </c>
-      <c r="L6" s="15">
-        <v>1.54</v>
-      </c>
-      <c r="M6" s="15">
-        <v>1.43</v>
-      </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="8">
-        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
-        <v>127.32395461900511</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="15">
-        <f>2-((H5)/2-1)*0.1</f>
-        <v>2</v>
-      </c>
-      <c r="I7" s="15">
-        <f>2-((I5)/2-1)*0.115</f>
-        <v>1.885</v>
-      </c>
-      <c r="J7" s="15">
-        <f t="shared" ref="J7:M7" si="0">2-((J5)/2-1)*0.115</f>
-        <v>1.77</v>
-      </c>
-      <c r="K7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.655</v>
-      </c>
-      <c r="L7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-      <c r="M7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.4249999999999998</v>
-      </c>
-      <c r="N7" s="15">
-        <f>2-((N5)/2-1)*0.11</f>
-        <v>1.3399999999999999</v>
-      </c>
-      <c r="O7" s="15">
-        <f t="shared" ref="O7:Q7" si="1">2-((O5)/2-1)*0.11</f>
-        <v>1.23</v>
-      </c>
-      <c r="P7" s="15">
-        <f t="shared" si="1"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q7" s="15">
-        <f t="shared" si="1"/>
-        <v>1.01</v>
-      </c>
-      <c r="R7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="8">
-        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
-        <v>2127.6595744680853</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="7">
-        <f>Parameters!C3/Parameters!C5</f>
-        <v>270</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="8">
-        <f>0.612*Parameters!C6*C9/SQRT(3)</f>
-        <v>81.091154708759703</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="8">
-        <f>C8/(Parameters!G3*Calculations!C10*3)</f>
-        <v>9.7177314523144265</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="7">
-        <f>Parameters!C8*Calculations!C4/120</f>
-        <v>100</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="7">
-        <f>Parameters!C11*Parameters!C12</f>
-        <v>45</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="10">
-        <f>2*C7/(C13*1000*Parameters!G8)</f>
-        <v>1.8012654910913857E-3</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14">
-        <f>0.155^2*150</f>
-        <v>3.6037500000000002</v>
-      </c>
-      <c r="K14">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="11">
-        <f>1000*(C14/C15)^(1/3)</f>
-        <v>181.7546335652992</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="11">
-        <f>C16*C15</f>
-        <v>54.526390069589759</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="11">
-        <f>C18*C16</f>
-        <v>254.45648699141887</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="7">
-        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="8">
-        <f>Parameters!G8*Calculations!C16/Calculations!C3</f>
-        <v>23.791625871341139</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="16">
-        <f>0.001*2*C16*C17*Parameters!C12/Calculations!C4</f>
-        <v>0.891938164206317</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="7">
-        <v>100</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="7">
-        <f>C23*Parameters!C9*Parameters!C15/2</f>
-        <v>200</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="8">
-        <f>4.44*C24*C12*C22*C6/1000</f>
-        <v>73.897433679759047</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C19" sqref="A1:C19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,82 +2882,177 @@
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="12">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12">
+        <v>4</v>
+      </c>
+      <c r="D1" s="12">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12">
+        <v>10</v>
+      </c>
+      <c r="G1" s="12">
+        <v>12</v>
+      </c>
+      <c r="H1" s="12">
+        <v>14</v>
+      </c>
+      <c r="I1" s="12">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12">
+        <v>18</v>
+      </c>
+      <c r="K1" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1.88</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1.78</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1.66</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1.54</v>
+      </c>
+      <c r="G2" s="14">
+        <v>1.43</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="14">
+        <f>2-((B1)/2-1)*0.1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <f>2-((C1)/2-1)*0.115</f>
+        <v>1.885</v>
+      </c>
+      <c r="D3" s="14">
+        <f>2-((D1)/2-1)*0.115</f>
+        <v>1.77</v>
+      </c>
+      <c r="E3" s="14">
+        <f>2-((E1)/2-1)*0.115</f>
+        <v>1.655</v>
+      </c>
+      <c r="F3" s="14">
+        <f>2-((F1)/2-1)*0.115</f>
+        <v>1.54</v>
+      </c>
+      <c r="G3" s="14">
+        <f>2-((G1)/2-1)*0.115</f>
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="H3" s="14">
+        <f>2-((H1)/2-1)*0.11</f>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="I3" s="14">
+        <f>2-((I1)/2-1)*0.11</f>
+        <v>1.23</v>
+      </c>
+      <c r="J3" s="14">
+        <f>2-((J1)/2-1)*0.11</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K3" s="14">
+        <f>2-((K1)/2-1)*0.11</f>
+        <v>1.01</v>
+      </c>
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
Design files: Efficiency added. Comparison with maxwell results is implemented. There is a huge error which is caused by the series-parallel connection of the modules.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Designfile.xlsx
+++ b/Project/BAP/Design/Designfile.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mesutto\Desktop\github work\immd\Project\BAP\Design\"/>
@@ -26,8 +26,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>mesutto</author>
+  </authors>
+  <commentList>
+    <comment ref="H5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+AWG#13</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="180">
   <si>
     <t>Power factor</t>
   </si>
@@ -699,9 +735,6 @@
     <t>Stator slot pitch</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Flux per pole</t>
   </si>
   <si>
@@ -882,17 +915,491 @@
   </si>
   <si>
     <t>δ</t>
+  </si>
+  <si>
+    <t>Required copper diameter</t>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>Selected copper diameter</t>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu-req</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>sp</t>
+    </r>
+  </si>
+  <si>
+    <t>Copper area per slot</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Winding</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Ω/km</t>
+  </si>
+  <si>
+    <t>Φpp</t>
+  </si>
+  <si>
+    <t>Induced voltage</t>
+  </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s2</t>
+    </r>
+  </si>
+  <si>
+    <t>Slot height - 2</t>
+  </si>
+  <si>
+    <t>Slot height - 1</t>
+  </si>
+  <si>
+    <t>Slot height - 0</t>
+  </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s0</t>
+    </r>
+  </si>
+  <si>
+    <t>Back core height</t>
+  </si>
+  <si>
+    <r>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>bc</t>
+    </r>
+  </si>
+  <si>
+    <t>Slot width - 0</t>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s2</t>
+    </r>
+  </si>
+  <si>
+    <t>Slot width - 2</t>
+  </si>
+  <si>
+    <t>Slot width - 1</t>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s0</t>
+    </r>
+  </si>
+  <si>
+    <t>Induced voltage (module-ph)</t>
+  </si>
+  <si>
+    <t>Wire specific resistance</t>
+  </si>
+  <si>
+    <t>Tooth width</t>
+  </si>
+  <si>
+    <t>Smooth edge</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>t</t>
+    </r>
+  </si>
+  <si>
+    <t>Stator slot end pitch</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>se</t>
+    </r>
+  </si>
+  <si>
+    <t>Slot area</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>kcu</t>
+  </si>
+  <si>
+    <t>Magnet embrace</t>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Ind voltage</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Scaled</t>
+  </si>
+  <si>
+    <t>Error (%)</t>
+  </si>
+  <si>
+    <t>Elect. Loading</t>
+  </si>
+  <si>
+    <t>Current Density</t>
+  </si>
+  <si>
+    <r>
+      <t>A/mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Copper length</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase resistance</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>ph</t>
+    </r>
+  </si>
+  <si>
+    <t>mΩ</t>
+  </si>
+  <si>
+    <t>Phase copper loss</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu-ph</t>
+    </r>
+  </si>
+  <si>
+    <t>Total loss</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -941,6 +1448,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Garamond"/>
@@ -954,6 +1470,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1003,19 +1543,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1049,11 +1576,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1098,23 +1634,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1131,6 +1651,69 @@
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1412,30 +1995,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -1448,20 +2033,21 @@
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1474,20 +2060,21 @@
       <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="7">
+      <c r="H2" s="7">
         <v>94</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1500,21 +2087,22 @@
       <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>0.9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1527,20 +2115,21 @@
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>98</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1553,10 +2142,15 @@
       <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1569,10 +2163,15 @@
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1585,16 +2184,17 @@
       <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1607,18 +2207,19 @@
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>3.1415926500000002</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1631,20 +2232,21 @@
       <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="25">
+        <v>1.7E-8</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="31">
-        <v>1.7E-8</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1657,20 +2259,21 @@
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="30" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1.2566289999999999E-6</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="31">
-        <v>1.2566289999999999E-6</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1683,12 +2286,13 @@
       <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
@@ -1701,12 +2305,13 @@
       <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1719,12 +2324,13 @@
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>89</v>
       </c>
@@ -1732,21 +2338,25 @@
         <v>90</v>
       </c>
       <c r="C14" s="7">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="C15" s="7">
         <v>2</v>
@@ -1754,14 +2364,41 @@
       <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1769,46 +2406,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="21" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -1835,8 +2497,37 @@
         <v>6</v>
       </c>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="U2" s="12"/>
+    </row>
+    <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1851,22 +2542,54 @@
         <v>15</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="8">
+        <f>1000*SQRT(2*Parameters!H9/(2*Parameters!H8*M8*Parameters!H10))</f>
+        <v>6.562147464226471</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="7">
+      <c r="M3" s="7">
         <f>Parameters!C4/Parameters!C5</f>
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="28"/>
-    </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="22"/>
+      <c r="P3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="41">
+        <v>55.77</v>
+      </c>
+      <c r="S3" s="42">
+        <f>R3/(2)</f>
+        <v>27.885000000000002</v>
+      </c>
+      <c r="T3" s="42">
+        <f>100*ABS(S3-M7)/M7</f>
+        <v>186.94968714492271</v>
+      </c>
+      <c r="U3" s="41"/>
+    </row>
+    <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1881,22 +2604,54 @@
         <v>15</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="8">
+        <f>SQRT(4*M7/(Parameters!H8*Parameters!C13))</f>
+        <v>1.7587637692667544</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="10">
-        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
+      <c r="M4" s="10">
+        <f>Parameters!C2/(Parameters!C4*Parameters!H2/100)</f>
         <v>2127.6595744680853</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="28"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="22"/>
+      <c r="P4" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="41">
+        <v>121.5</v>
+      </c>
+      <c r="S4" s="42">
+        <f>R4/(2*SQRT(2)*SQRT(3))</f>
+        <v>24.801083645679675</v>
+      </c>
+      <c r="T4" s="42">
+        <f>100*ABS(H15-S4)/H15</f>
+        <v>5.6437955509280773</v>
+      </c>
+      <c r="U4" s="43"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -1911,271 +2666,509 @@
         <v>15</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1.8288</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="7">
+      <c r="M5" s="7">
         <f>Parameters!C3/Parameters!C5</f>
         <v>270</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="22"/>
+      <c r="P5" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q5" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="41">
+        <v>83.546999999999997</v>
+      </c>
+      <c r="S5" s="41">
+        <v>83.546999999999997</v>
+      </c>
+      <c r="T5" s="42">
+        <f>100*ABS(Parameters!C11-S5)/Parameters!C11</f>
+        <v>67.093999999999994</v>
+      </c>
+      <c r="U5" s="41"/>
+    </row>
+    <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C6" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="8">
-        <f>0.612*Parameters!C6*H5/SQRT(3)</f>
-        <v>81.091154708759703</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="7">
         <f>Parameters!C11*Parameters!C12</f>
         <v>45</v>
       </c>
+      <c r="D6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="8">
+        <v>6.5698400000000001</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="26"/>
+      <c r="K6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="8">
+        <f>0.612*Parameters!C6*M5/SQRT(3)</f>
+        <v>81.091154708759703</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="21"/>
+      <c r="P6" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q6" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="R6" s="41">
+        <v>10.63</v>
+      </c>
+      <c r="S6" s="41">
+        <v>10.63</v>
+      </c>
+      <c r="T6" s="42">
+        <f>100*ABS(Parameters!C13-S6)/Parameters!C13</f>
+        <v>165.75000000000003</v>
+      </c>
+      <c r="U6" s="41"/>
+    </row>
+    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8">
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!H8/60)</f>
+        <v>127.32395461900511</v>
+      </c>
       <c r="D7" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="8">
+        <f>Parameters!C15*H13*Parameters!H8*(H5*1.02/2)^2</f>
+        <v>163.97358840077737</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="8">
-        <f>H4/(Parameters!G3*'General Calculations'!H6*3)</f>
+      <c r="M7" s="8">
+        <f>M4/(Parameters!H3*'General Calculations'!M6*3)</f>
         <v>9.7177314523144265</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="22"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="42">
+        <f t="shared" ref="T5:T9" si="0">100*ABS(H18-S7)/H18</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="U7" s="41"/>
+    </row>
+    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="8">
-        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
-        <v>127.32395461900511</v>
+        <v>75</v>
+      </c>
+      <c r="C8" s="9">
+        <f>2*C7/(C6*1000*Parameters!H8)</f>
+        <v>1.8012654910913857E-3</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="28"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="7">
+      <c r="M8" s="7">
         <f>Parameters!C8*'General Calculations'!C4/120</f>
         <v>100</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="22"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="42">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="U8" s="41"/>
+    </row>
+    <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="9">
-        <f>2*C8/(C7*1000*Parameters!G8)</f>
-        <v>1.8012654910913857E-3</v>
+        <v>78</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="42">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="U9" s="41"/>
+    </row>
+    <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.3</v>
+        <v>80</v>
+      </c>
+      <c r="C10" s="10">
+        <f>1000*(C8/C9)^(1/3)</f>
+        <v>153.29779501892307</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="10">
+        <f>C10*C9</f>
+        <v>76.648897509461534</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="J11" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="M11" s="32">
+        <v>17</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="20">
-        <f>1000*(C9/C10)^(1/3)</f>
-        <v>181.7546335652992</v>
-      </c>
-      <c r="D11" s="19" t="s">
+    </row>
+    <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="15">
+        <f>0.001*2*C10*C11*Parameters!C12/'General Calculations'!C4</f>
+        <v>1.0575096280948688</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" s="32">
+        <v>2</v>
+      </c>
+      <c r="N12" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26"/>
-    </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="10">
-        <f>C11*C10</f>
-        <v>54.526390069589759</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="O12" s="26"/>
+    </row>
+    <row r="13" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="10">
+        <f>C12*C10</f>
+        <v>214.61691302649228</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="7">
+        <v>30</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="27"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K13" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" s="32">
+        <v>2</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="26"/>
+    </row>
+    <row r="14" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="10">
-        <f>C13*C11</f>
-        <v>254.45648699141887</v>
+        <v>87</v>
+      </c>
+      <c r="C14" s="7">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="26"/>
-    </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="21"/>
+      <c r="F14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="7">
+        <f>H13*Parameters!C9*Parameters!C15/2</f>
+        <v>60</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="M14" s="36">
+        <f>C13/2-C10/2-M11-M12-M13-M19</f>
+        <v>7.659559003784608</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="33"/>
+    </row>
+    <row r="15" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="7">
-        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
-        <v>0.6</v>
+        <v>95</v>
+      </c>
+      <c r="C15" s="8">
+        <f>Parameters!H8*C10/'General Calculations'!C3</f>
+        <v>20.066634420527304</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="27"/>
-    </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="8">
+        <f>4.44*H12*M8*H14*H11/1000</f>
+        <v>26.28452870745334</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="L15" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="35">
+        <v>8</v>
+      </c>
+      <c r="N15" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="C16" s="8">
-        <f>Parameters!G8*C11/'General Calculations'!C3</f>
-        <v>23.791625871341139</v>
+        <f>Parameters!H8*(C13-M14)/'General Calculations'!C3</f>
+        <v>27.090654260882769</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>81</v>
@@ -2185,151 +3178,237 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="15">
-        <f>0.001*2*C11*C12*Parameters!C12/'General Calculations'!C4</f>
-        <v>0.891938164206317</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>98</v>
-      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="M16" s="36">
+        <f>C16-M15</f>
+        <v>19.090654260882769</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" s="33"/>
+    </row>
+    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="7">
-        <v>100</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="F17" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="M17" s="36">
+        <f>C15-M15</f>
+        <v>12.066634420527304</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O17" s="33"/>
+    </row>
+    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="8">
+        <f>2*Parameters!C9*C11*1.2</f>
+        <v>367.91470804541535</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="M18" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="32"/>
+    </row>
+    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H19" s="8">
+        <f>H18*H6/(H13)</f>
+        <v>80.571358850169716</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="M19" s="32">
+        <v>2</v>
+      </c>
+      <c r="N19" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="7">
+        <f>M7^2*H19/1000</f>
+        <v>7.6087002420250913</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="M20" s="8">
+        <f>(M16+M17)*M11/2</f>
+        <v>264.83695379198559</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O20" s="32"/>
+    </row>
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" s="7">
+        <f>H20*Parameters!C4*Parameters!C7</f>
+        <v>91.304402904301099</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="M21" s="8">
+        <f>H7/M20</f>
+        <v>0.61914920124617245</v>
+      </c>
+      <c r="N21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="7">
-        <f>C18*Parameters!C9*Parameters!C15/2</f>
-        <v>200</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="7">
+        <f>Parameters!C2/(Parameters!C2+'General Calculations'!H21)*100</f>
+        <v>98.871573749326146</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="8">
-        <f>4.44*C19*H8*C17*C6/1000</f>
-        <v>73.897433679759047</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="8">
-        <f>1000*SQRT(2*Parameters!G9/(2*Parameters!G8*H8*Parameters!G10))</f>
-        <v>6.562147464226471</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="3"/>
-    </row>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="19"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F17:J17"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="O11:O13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -2504,7 +3583,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="8">
-        <f>Parameters!C2/(Parameters!C8*2*Parameters!G8/60)</f>
+        <f>Parameters!C2/(Parameters!C8*2*Parameters!H8/60)</f>
         <v>127.32395461900511</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -2554,7 +3633,7 @@
         <v>1.01</v>
       </c>
       <c r="R7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -2565,7 +3644,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="8">
-        <f>Parameters!C2/(Parameters!C4*Parameters!G2/100)</f>
+        <f>Parameters!C2/(Parameters!C4*Parameters!H2/100)</f>
         <v>2127.6595744680853</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -2610,7 +3689,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="8">
-        <f>C8/(Parameters!G3*'Calculations-old'!C10*3)</f>
+        <f>C8/(Parameters!H3*'Calculations-old'!C10*3)</f>
         <v>9.7177314523144265</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -2655,7 +3734,7 @@
         <v>75</v>
       </c>
       <c r="C14" s="9">
-        <f>2*C7/(C13*1000*Parameters!G8)</f>
+        <f>2*C7/(C13*1000*Parameters!H8)</f>
         <v>1.8012654910913857E-3</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -2773,10 +3852,10 @@
         <v>93</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="8">
-        <f>Parameters!G8*'Calculations-old'!C16/'Calculations-old'!C3</f>
+        <f>Parameters!H8*'Calculations-old'!C16/'Calculations-old'!C3</f>
         <v>23.791625871341139</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -2785,25 +3864,25 @@
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="15">
         <f>0.001*2*C16*C17*Parameters!C12/'Calculations-old'!C4</f>
         <v>0.891938164206317</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="7">
         <v>100</v>
@@ -2814,10 +3893,10 @@
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="C24" s="7">
         <f>C23*Parameters!C9*Parameters!C15/2</f>
@@ -2829,10 +3908,10 @@
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="C25" s="8">
         <f>4.44*C24*C12*C22*C6/1000</f>
@@ -2871,6 +3950,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -2989,7 +4069,7 @@
         <v>1.01</v>
       </c>
       <c r="L3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Studies on magnet, flux density etc. Design file is currently a fail, still working on it.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Designfile.xlsx
+++ b/Project/BAP/Design/Designfile.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="219">
   <si>
     <t>Power factor</t>
   </si>
@@ -845,9 +845,6 @@
     <t>Drive</t>
   </si>
   <si>
-    <t>Inh</t>
-  </si>
-  <si>
     <t>Copper resistivity</t>
   </si>
   <si>
@@ -1264,12 +1261,6 @@
     <t>Maxwell</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Ind voltage</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -1288,118 +1279,412 @@
     <t>Current Density</t>
   </si>
   <si>
-    <r>
-      <t>A/mm</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Copper length</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase resistance</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>ph</t>
+    </r>
+  </si>
+  <si>
+    <t>mΩ</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>cu-ph</t>
+    </r>
+  </si>
+  <si>
+    <t>Total loss</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Analytic</t>
+  </si>
+  <si>
+    <t>Copper loss</t>
+  </si>
+  <si>
+    <t>Line current (m-p)</t>
+  </si>
+  <si>
+    <t>Ind voltage (m-p)</t>
+  </si>
+  <si>
+    <t>Arms</t>
+  </si>
+  <si>
+    <t>Vrms</t>
+  </si>
+  <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>Fill factor</t>
+  </si>
+  <si>
+    <t>pwt</t>
+  </si>
+  <si>
+    <t>inh</t>
+  </si>
+  <si>
+    <t>Core loss</t>
+  </si>
+  <si>
+    <t>Copper loss/module/phase</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>loss</t>
+    </r>
+  </si>
+  <si>
+    <t>Half turn length</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Magnet</t>
+  </si>
+  <si>
+    <t>Air gap effective pole area</t>
+  </si>
+  <si>
+    <t>Magnet effective pole area</t>
+  </si>
+  <si>
+    <t>Magnet relative permeability</t>
+  </si>
+  <si>
+    <t>Air permeability</t>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="162"/>
-        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>Magnet permeability</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>rm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>rec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>η</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>Magnet pole angle</t>
+  </si>
+  <si>
+    <r>
+      <t>θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <r>
+      <t>cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
       </rPr>
       <t>2</t>
     </r>
   </si>
   <si>
-    <t>Loss</t>
-  </si>
-  <si>
-    <t>Copper length</t>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>cu</t>
-    </r>
-  </si>
-  <si>
-    <t>Phase resistance</t>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>ph</t>
-    </r>
-  </si>
-  <si>
-    <t>mΩ</t>
-  </si>
-  <si>
-    <t>Phase copper loss</t>
-  </si>
-  <si>
-    <r>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>cu-ph</t>
-    </r>
-  </si>
-  <si>
-    <t>Total loss</t>
-  </si>
-  <si>
-    <r>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>cu</t>
-    </r>
-  </si>
-  <si>
-    <t>Efficiency</t>
+    <t>Flux concentration coefficient</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+  </si>
+  <si>
+    <t>Permeance Coefficient</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Remanent flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <t>Air gep flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r1</t>
+    </r>
+  </si>
+  <si>
+    <t>Magnet leakage coefficient</t>
+  </si>
+  <si>
+    <t>Carter's coefficient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1447,23 +1732,6 @@
       <charset val="162"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Garamond"/>
-      <family val="1"/>
-      <charset val="162"/>
-    </font>
-    <font>
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1487,13 +1755,21 @@
       <charset val="162"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="162"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1580,16 +1856,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1634,86 +1914,119 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1999,7 +2312,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,12 +2498,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -2234,16 +2547,16 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="19">
+        <v>1.7E-8</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="25">
-        <v>1.7E-8</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.35">
@@ -2261,16 +2574,16 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1.2566289999999999E-6</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H10" s="25">
-        <v>1.2566289999999999E-6</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.35">
@@ -2287,10 +2600,19 @@
         <v>23</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="F11" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11" s="19">
+        <f>4*H8*0.0000001</f>
+        <v>1.2566370599999999E-6</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -2344,7 +2666,7 @@
         <v>81</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -2372,10 +2694,10 @@
     </row>
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="C16" s="7">
         <v>0.7</v>
@@ -2384,7 +2706,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
@@ -2408,989 +2730,1418 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7" style="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="23" max="29" width="4.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="38" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+    </row>
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="31"/>
+      <c r="P2" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-    </row>
-    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="Q2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="37" t="s">
+      <c r="R2" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="T2" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="U2" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="Q2" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="S2" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="T2" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="U2" s="12"/>
-    </row>
-    <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="V2" s="21"/>
+    </row>
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="21">
         <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="28" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="8">
+      <c r="H3" s="24">
         <f>1000*SQRT(2*Parameters!H9/(2*Parameters!H8*M8*Parameters!H10))</f>
         <v>6.562147464226471</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="35"/>
+      <c r="K3" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="21">
         <f>Parameters!C4/Parameters!C5</f>
         <v>2</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="41">
-        <v>55.77</v>
-      </c>
-      <c r="S3" s="42">
-        <f>R3/(2)</f>
-        <v>27.885000000000002</v>
-      </c>
-      <c r="T3" s="42">
-        <f>100*ABS(S3-M7)/M7</f>
-        <v>186.94968714492271</v>
-      </c>
-      <c r="U3" s="41"/>
-    </row>
-    <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="O3" s="37"/>
+      <c r="P3" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="R3" s="24">
+        <v>15</v>
+      </c>
+      <c r="S3" s="24">
+        <f>R3</f>
+        <v>15</v>
+      </c>
+      <c r="T3" s="24">
+        <f>M7</f>
+        <v>9.7177314523144265</v>
+      </c>
+      <c r="U3" s="24">
+        <f>100*ABS(S3-T3)/T3</f>
+        <v>54.357012988124097</v>
+      </c>
+      <c r="V3" s="21"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="21">
         <f>Parameters!C9*10</f>
         <v>20</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="E4" s="31"/>
+      <c r="F4" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="24">
         <f>SQRT(4*M7/(Parameters!H8*Parameters!C13))</f>
         <v>1.7587637692667544</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="39">
         <f>Parameters!C2/(Parameters!C4*Parameters!H2/100)</f>
         <v>2127.6595744680853</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="41">
-        <v>121.5</v>
-      </c>
-      <c r="S4" s="42">
-        <f>R4/(2*SQRT(2)*SQRT(3))</f>
-        <v>24.801083645679675</v>
-      </c>
-      <c r="T4" s="42">
-        <f>100*ABS(H15-S4)/H15</f>
-        <v>5.6437955509280773</v>
-      </c>
-      <c r="U4" s="43"/>
-    </row>
-    <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="O4" s="37"/>
+      <c r="P4" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="R4" s="24">
+        <v>557</v>
+      </c>
+      <c r="S4" s="24">
+        <f>R4/(4*SQRT(2)*SQRT(3))</f>
+        <v>56.848574447092922</v>
+      </c>
+      <c r="T4" s="24">
+        <f>H15</f>
+        <v>67.108824000000027</v>
+      </c>
+      <c r="U4" s="24">
+        <f t="shared" ref="U4:U12" si="0">100*ABS(S4-T4)/T4</f>
+        <v>15.288972360634871</v>
+      </c>
+      <c r="V4" s="22"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="21">
         <f>C3/(C4*Parameters!C7)</f>
         <v>0.4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="E5" s="31"/>
+      <c r="F5" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="8">
+      <c r="G5" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="24">
         <v>1.8288</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="21" t="s">
         <v>81</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K5" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="21">
         <f>Parameters!C3/Parameters!C5</f>
         <v>270</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q5" s="41" t="s">
+      <c r="O5" s="37"/>
+      <c r="P5" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="41">
-        <v>83.546999999999997</v>
-      </c>
-      <c r="S5" s="41">
-        <v>83.546999999999997</v>
-      </c>
-      <c r="T5" s="42">
-        <f>100*ABS(Parameters!C11-S5)/Parameters!C11</f>
-        <v>67.093999999999994</v>
-      </c>
-      <c r="U5" s="41"/>
-    </row>
-    <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="R5" s="24">
+        <v>62.21</v>
+      </c>
+      <c r="S5" s="24">
+        <f>R5</f>
+        <v>62.21</v>
+      </c>
+      <c r="T5" s="24">
+        <f>Parameters!C11</f>
+        <v>50</v>
+      </c>
+      <c r="U5" s="24">
+        <f t="shared" si="0"/>
+        <v>24.42</v>
+      </c>
+      <c r="V5" s="21"/>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="21">
         <f>Parameters!C11*Parameters!C12</f>
         <v>45</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="E6" s="31"/>
+      <c r="F6" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="24">
         <v>6.5698400000000001</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>128</v>
+      <c r="I6" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="J6" s="26"/>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="24">
         <f>0.612*Parameters!C6*M5/SQRT(3)</f>
         <v>81.091154708759703</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q6" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="R6" s="41">
-        <v>10.63</v>
-      </c>
-      <c r="S6" s="41">
-        <v>10.63</v>
-      </c>
-      <c r="T6" s="42">
-        <f>100*ABS(Parameters!C13-S6)/Parameters!C13</f>
-        <v>165.75000000000003</v>
-      </c>
-      <c r="U6" s="41"/>
-    </row>
-    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="O6" s="22"/>
+      <c r="P6" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="24">
+        <v>4.75</v>
+      </c>
+      <c r="S6" s="24">
+        <f>R6</f>
+        <v>4.75</v>
+      </c>
+      <c r="T6" s="24">
+        <f>Parameters!C13</f>
+        <v>4</v>
+      </c>
+      <c r="U6" s="24">
+        <f t="shared" si="0"/>
+        <v>18.75</v>
+      </c>
+      <c r="V6" s="21"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="24">
         <f>Parameters!C2/(Parameters!C8*2*Parameters!H8/60)</f>
         <v>127.32395461900511</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="28" t="s">
+      <c r="E7" s="31"/>
+      <c r="F7" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="24">
+        <f>Parameters!C15*H13*Parameters!H8*(H5/2)^2*1.25</f>
+        <v>197.00786764799284</v>
+      </c>
+      <c r="I7" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="8">
-        <f>Parameters!C15*H13*Parameters!H8*(H5*1.02/2)^2</f>
-        <v>163.97358840077737</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="24">
         <f>M4/(Parameters!H3*'General Calculations'!M6*3)</f>
         <v>9.7177314523144265</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="42">
-        <f t="shared" ref="T5:T9" si="0">100*ABS(H18-S7)/H18</f>
-        <v>99.999999999999986</v>
-      </c>
-      <c r="U7" s="41"/>
-    </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="O7" s="37"/>
+      <c r="P7" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="24">
+        <v>351.3</v>
+      </c>
+      <c r="S7" s="24">
+        <f>R7</f>
+        <v>351.3</v>
+      </c>
+      <c r="T7" s="24">
+        <f>H22</f>
+        <v>178.68046222001527</v>
+      </c>
+      <c r="U7" s="24">
+        <f t="shared" si="0"/>
+        <v>96.607953457962566</v>
+      </c>
+      <c r="V7" s="21"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="40">
         <f>2*C7/(C6*1000*Parameters!H8)</f>
         <v>1.8012654910913857E-3</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="6" t="s">
+      <c r="E8" s="31"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="21">
         <f>Parameters!C8*'General Calculations'!C4/120</f>
         <v>100</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="42">
+      <c r="O8" s="37"/>
+      <c r="P8" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="24">
+        <f>21</f>
+        <v>21</v>
+      </c>
+      <c r="S8" s="24">
+        <f>R8</f>
+        <v>21</v>
+      </c>
+      <c r="T8" s="24">
+        <f>C7</f>
+        <v>127.32395461900511</v>
+      </c>
+      <c r="U8" s="24">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="U8" s="41"/>
-    </row>
-    <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+        <v>83.506638587500007</v>
+      </c>
+      <c r="V8" s="21"/>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="21">
         <v>0.5</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="42">
+      <c r="E9" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="24">
+        <f>1.26</f>
+        <v>1.26</v>
+      </c>
+      <c r="S9" s="24">
+        <f>R9</f>
+        <v>1.26</v>
+      </c>
+      <c r="T9" s="24">
+        <f>M21</f>
+        <v>0.5195961563928515</v>
+      </c>
+      <c r="U9" s="24">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="U9" s="41"/>
-    </row>
-    <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+        <v>142.49602012978534</v>
+      </c>
+      <c r="V9" s="21"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="39">
+        <v>200</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="R10" s="42">
+        <v>105.62</v>
+      </c>
+      <c r="S10" s="24">
+        <f>R10</f>
+        <v>105.62</v>
+      </c>
+      <c r="T10" s="24">
+        <f>C11+C16</f>
+        <v>184.42661945624999</v>
+      </c>
+      <c r="U10" s="24">
+        <f t="shared" si="0"/>
+        <v>42.730609978428106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="39">
+        <v>150</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="43"/>
+      <c r="F11" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="M11" s="21">
+        <v>17</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="P11" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="R11" s="42">
+        <f>0.6986*1000</f>
+        <v>698.6</v>
+      </c>
+      <c r="S11" s="42">
+        <f>R11/4</f>
+        <v>174.65</v>
+      </c>
+      <c r="T11" s="24">
+        <f>H19</f>
+        <v>157.67616000000001</v>
+      </c>
+      <c r="U11" s="24">
+        <f t="shared" si="0"/>
+        <v>10.765000872674724</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="44">
+        <f>0.001*2*C10*C11*Parameters!C12/C4</f>
+        <v>2.7</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" s="21">
+        <v>2</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" s="26"/>
+      <c r="P12" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="44">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="S12" s="44">
+        <f>R12</f>
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="T12" s="44">
+        <f>H11</f>
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="U12" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="39">
+        <f>C12*C10</f>
+        <v>280</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="21">
+        <v>30</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="21">
+        <v>2</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="26"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="21">
+        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="21">
+        <f>H13*Parameters!C9*Parameters!C15/2</f>
+        <v>60</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="M14" s="24">
+        <f>C13/2-C10/2-M11-M12-M13-M19</f>
+        <v>17</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="22"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="24">
+        <f>Parameters!H8*C10/'General Calculations'!C3</f>
+        <v>26.179938750000002</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="24">
+        <f>4.44*H12*M8*H14*H11/1000</f>
+        <v>67.108824000000027</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="43"/>
+      <c r="K15" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="M15" s="23">
+        <v>8</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="24">
+        <f>Parameters!H8*(C13-M14)/'General Calculations'!C3</f>
+        <v>34.426619456250002</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="M16" s="24">
+        <f>C16-M15</f>
+        <v>26.426619456250002</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" s="22"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="M17" s="24">
+        <f>C15-M15</f>
+        <v>18.179938750000002</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O17" s="22"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="24">
+        <f>2*Parameters!C9*C11*1.2</f>
+        <v>720</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="48"/>
+      <c r="K18" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="M18" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="21"/>
+      <c r="R18" s="45">
+        <f>80*4*SQRT(3)</f>
+        <v>554.25625842204067</v>
+      </c>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="24">
+        <f>H18*H6/(H13)</f>
+        <v>157.67616000000001</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="M19" s="21">
+        <v>2</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="39">
         <f>1000*(C8/C9)^(1/3)</f>
         <v>153.29779501892307</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D20" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-    </row>
-    <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="E20" s="46"/>
+      <c r="F20" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" s="21">
+        <f>M7^2*H19/1000</f>
+        <v>14.890038518334606</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="M20" s="24">
+        <f>(M16+M17)*M11/2</f>
+        <v>379.15574475312502</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="O20" s="21"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B21" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C21" s="39">
         <f>C10*C9</f>
-        <v>76.648897509461534</v>
-      </c>
-      <c r="D11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="28" t="s">
+      <c r="E21" s="46"/>
+      <c r="F21" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="21"/>
+      <c r="K21" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="M21" s="24">
+        <f>H7/M20</f>
+        <v>0.5195961563928515</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="21"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="21">
+        <f>H20*Parameters!C4*Parameters!C7+H21</f>
+        <v>178.68046222001527</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="21">
+        <f>Parameters!C2/(Parameters!C2+'General Calculations'!H22)*100</f>
+        <v>97.815289849684206</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="54"/>
+      <c r="K23" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="L24" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="M24" s="44">
+        <f>2*Parameters!H8*Parameters!C16/'General Calculations'!C4</f>
+        <v>0.2199114855</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="O24" s="21"/>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="52"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="L25" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="M25" s="21">
+        <f>M24*180/Parameters!H8</f>
+        <v>12.6</v>
+      </c>
+      <c r="N25" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="O25" s="21"/>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="52"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="L26" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="M26" s="24">
+        <f>(M24*(C10/2-C14/2)+2*C14)*(C11+2*C14)/100</f>
+        <v>34.965264757777192</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="35"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="L27" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="M27" s="24">
+        <f>(M24*(C10/2-C14/2-Parameters!C14/2)+2*C14)*(C11)/100</f>
+        <v>34.110495007087501</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="O27" s="21"/>
+    </row>
+    <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="L28" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="M28" s="24">
+        <f>M27/M26</f>
+        <v>0.97555374579282805</v>
+      </c>
+      <c r="N28" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O28" s="21"/>
+    </row>
+    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="H29" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="51"/>
+      <c r="K29" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="L29" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="M29" s="24">
+        <f>M27*C14/(M26*Parameters!C14)</f>
+        <v>0.16723778499305625</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O29" s="21"/>
+    </row>
+    <row r="30" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H30" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="51"/>
+      <c r="K30" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="M30" s="21">
+        <v>1000</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="36"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="L31" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="M31" s="55">
+        <f>M30*Parameters!H11</f>
+        <v>1.2566370599999999E-3</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="O31" s="21"/>
+    </row>
+    <row r="32" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="F32" s="36"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="L32" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="M32" s="24">
         <v>1</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="M11" s="32">
-        <v>17</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O11" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" s="15">
-        <f>0.001*2*C10*C11*Parameters!C12/'General Calculations'!C4</f>
-        <v>1.0575096280948688</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="M12" s="32">
-        <v>2</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O12" s="26"/>
-    </row>
-    <row r="13" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="10">
-        <f>C12*C10</f>
-        <v>214.61691302649228</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="7">
-        <v>30</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="M13" s="32">
-        <v>2</v>
-      </c>
-      <c r="N13" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O13" s="26"/>
-    </row>
-    <row r="14" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="7">
-        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H14" s="7">
-        <f>H13*Parameters!C9*Parameters!C15/2</f>
-        <v>60</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="M14" s="36">
-        <f>C13/2-C10/2-M11-M12-M13-M19</f>
-        <v>7.659559003784608</v>
-      </c>
-      <c r="N14" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O14" s="33"/>
-    </row>
-    <row r="15" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="8">
-        <f>Parameters!H8*C10/'General Calculations'!C3</f>
-        <v>20.066634420527304</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="8">
-        <f>4.44*H12*M8*H14*H11/1000</f>
-        <v>26.28452870745334</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="M15" s="35">
-        <v>8</v>
-      </c>
-      <c r="N15" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="O15" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="8">
-        <f>Parameters!H8*(C13-M14)/'General Calculations'!C3</f>
-        <v>27.090654260882769</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="M16" s="36">
-        <f>C16-M15</f>
-        <v>19.090654260882769</v>
-      </c>
-      <c r="N16" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O16" s="33"/>
-    </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="L17" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="M17" s="36">
-        <f>C15-M15</f>
-        <v>12.066634420527304</v>
-      </c>
-      <c r="N17" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O17" s="33"/>
-    </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="H18" s="8">
-        <f>2*Parameters!C9*C11*1.2</f>
-        <v>367.91470804541535</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="M18" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="N18" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O18" s="32"/>
-    </row>
-    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="H19" s="8">
-        <f>H18*H6/(H13)</f>
-        <v>80.571358850169716</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="L19" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="M19" s="32">
-        <v>2</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20" s="7">
-        <f>M7^2*H19/1000</f>
-        <v>7.6087002420250913</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="M20" s="8">
-        <f>(M16+M17)*M11/2</f>
-        <v>264.83695379198559</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="O20" s="32"/>
-    </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="H21" s="7">
-        <f>H20*Parameters!C4*Parameters!C7</f>
-        <v>91.304402904301099</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="M21" s="8">
-        <f>H7/M20</f>
-        <v>0.61914920124617245</v>
-      </c>
-      <c r="N21" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="7">
-        <f>Parameters!C2/(Parameters!C2+'General Calculations'!H21)*100</f>
-        <v>98.871573749326146</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="19"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="N32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O32" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="6:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="F33" s="36"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="M33" s="24">
+        <f>M28/(1+M30*M29*H29*(1+H30))</f>
+        <v>4.5896360150966195E-3</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="P1:U1"/>
+  <mergeCells count="10">
+    <mergeCell ref="K23:O23"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="K1:O1"/>
@@ -3399,6 +4150,7 @@
     <mergeCell ref="F10:J10"/>
     <mergeCell ref="K10:O10"/>
     <mergeCell ref="O11:O13"/>
+    <mergeCell ref="P1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Design file continue. Feedback is taken, design procedure will be re-visited.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Designfile.xlsx
+++ b/Project/BAP/Design/Designfile.xlsx
@@ -14,8 +14,8 @@
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="General Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="Calculations-old" sheetId="3" r:id="rId3"/>
-    <sheet name="Burdadursun" sheetId="2" r:id="rId4"/>
+    <sheet name="Figures" sheetId="5" r:id="rId3"/>
+    <sheet name="Not used-old" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,6 +27,70 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>mesutto</author>
+  </authors>
+  <commentList>
+    <comment ref="C12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+Note that this is peak air gap flux density, not average.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>mesutto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
+This is actually a design parameter.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>mesutto</author>
@@ -63,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="236">
   <si>
     <t>Power factor</t>
   </si>
@@ -483,9 +547,6 @@
     </r>
   </si>
   <si>
-    <t>Definitions</t>
-  </si>
-  <si>
     <t>pi</t>
   </si>
   <si>
@@ -1198,22 +1259,6 @@
     <t>Stator slot end pitch</t>
   </si>
   <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-        <charset val="162"/>
-      </rPr>
-      <t>se</t>
-    </r>
-  </si>
-  <si>
     <t>Slot area</t>
   </si>
   <si>
@@ -1253,12 +1298,6 @@
       </rPr>
       <t>m</t>
     </r>
-  </si>
-  <si>
-    <t>not used</t>
-  </si>
-  <si>
-    <t>Maxwell</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -1619,9 +1658,6 @@
     </r>
   </si>
   <si>
-    <t>Air gep flux density</t>
-  </si>
-  <si>
     <r>
       <t>B</t>
     </r>
@@ -1674,6 +1710,192 @@
   </si>
   <si>
     <t>Carter's coefficient</t>
+  </si>
+  <si>
+    <t>Slot fraction</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>uyd</t>
+  </si>
+  <si>
+    <t>Maxwell Results Comparison</t>
+  </si>
+  <si>
+    <t>Lakage factor</t>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>l</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <t>Reluctance factor</t>
+  </si>
+  <si>
+    <t>Air gap flux density</t>
+  </si>
+  <si>
+    <t>cns</t>
+  </si>
+  <si>
+    <t>Definitions - Constants</t>
+  </si>
+  <si>
+    <t>The electrical loading, magnetic loading and current density are selected as follows:</t>
+  </si>
+  <si>
+    <t>Average air gap flux density</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>se</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>avg</t>
+    </r>
+  </si>
+  <si>
+    <t>Circuit schematic for drive</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <t>Induced voltage (all-series)</t>
+  </si>
+  <si>
+    <r>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>ph</t>
+    </r>
+  </si>
+  <si>
+    <t>Peak Tooth Flux</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1906,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1771,8 +1993,26 @@
       <charset val="162"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1788,6 +2028,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1869,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1920,9 +2184,6 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1983,9 +2244,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2011,21 +2269,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2043,6 +2329,162 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>36634</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3216518</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="38680"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="36634" y="197827"/>
+          <a:ext cx="3179884" cy="2989385"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3282461</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6669551</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>39419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="34394"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3282461" y="307731"/>
+          <a:ext cx="3387090" cy="2596515"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>6850674</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>80597</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>356822</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>23447</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5121" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s5121"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2307,12 +2749,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2763,7 @@
     <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -2333,20 +2775,20 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
@@ -2360,20 +2802,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="20">
         <v>8000</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="6" t="s">
         <v>49</v>
       </c>
@@ -2387,20 +2829,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="20">
         <v>540</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2415,20 +2857,20 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="20">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="6" t="s">
         <v>53</v>
       </c>
@@ -2442,20 +2884,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="20">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -2463,20 +2905,22 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="20">
         <v>0.85</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="58" t="s">
+        <v>178</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -2484,46 +2928,46 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="20">
         <v>3</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="20">
         <v>600</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" s="8">
         <v>3.1415926500000002</v>
@@ -2532,182 +2976,182 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="20">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H9" s="19">
         <v>1.7E-8</v>
       </c>
       <c r="I9" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="G10" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H10" s="19">
         <v>1.2566289999999999E-6</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="20">
         <v>50</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H11" s="19">
         <f>4*H8*0.0000001</f>
         <v>1.2566370599999999E-6</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="20">
         <v>0.9</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="20">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="C14" s="20">
         <v>3.5</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>157</v>
+      <c r="D14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>178</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="C15" s="20">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="7">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="20">
         <v>0.7</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>157</v>
-      </c>
+      <c r="E16" s="21"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2724,6 +3168,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2732,1412 +3177,1471 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7" style="26" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="29" width="4.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="24.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7" style="25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="29" width="4.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="53" t="s">
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="24"/>
+    </row>
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="24"/>
+      <c r="P2" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="T2" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="25"/>
-    </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q2" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="S2" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="V2" s="21"/>
+      <c r="V2" s="20"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <f>Parameters!C4*Parameters!C7*Parameters!C9</f>
         <v>24</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <f>1000*SQRT(2*Parameters!H9/(2*Parameters!H8*M8*Parameters!H10))</f>
         <v>6.562147464226471</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29" t="s">
+      <c r="I3" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="20">
         <f>Parameters!C4/Parameters!C5</f>
         <v>2</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="R3" s="24">
+      <c r="O3" s="30"/>
+      <c r="P3" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="R3" s="23">
         <v>15</v>
       </c>
-      <c r="S3" s="24">
+      <c r="S3" s="23">
         <f>R3</f>
         <v>15</v>
       </c>
-      <c r="T3" s="24">
+      <c r="T3" s="23">
         <f>M7</f>
         <v>9.7177314523144265</v>
       </c>
-      <c r="U3" s="24">
+      <c r="U3" s="23">
         <f>100*ABS(S3-T3)/T3</f>
         <v>54.357012988124097</v>
       </c>
-      <c r="V3" s="21"/>
+      <c r="V3" s="20"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <f>Parameters!C9*10</f>
         <v>20</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="24">
+      <c r="E4" s="24"/>
+      <c r="F4" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="23">
         <f>SQRT(4*M7/(Parameters!H8*Parameters!C13))</f>
         <v>1.7587637692667544</v>
       </c>
-      <c r="I4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="29" t="s">
+      <c r="I4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="33">
+      <c r="M4" s="32">
         <f>Parameters!C2/(Parameters!C4*Parameters!H2/100)</f>
         <v>2127.6595744680853</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q4" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="R4" s="24">
+      <c r="O4" s="30"/>
+      <c r="P4" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" s="23">
         <v>557</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="23">
         <f>R4/(4*SQRT(2)*SQRT(3))</f>
         <v>56.848574447092922</v>
       </c>
-      <c r="T4" s="24">
+      <c r="T4" s="23">
         <f>H15</f>
-        <v>67.108824000000027</v>
-      </c>
-      <c r="U4" s="24">
+        <v>29.956922473408429</v>
+      </c>
+      <c r="U4" s="23">
         <f t="shared" ref="U4:U12" si="0">100*ABS(S4-T4)/T4</f>
-        <v>15.288972360634871</v>
-      </c>
-      <c r="V4" s="22"/>
+        <v>89.767738984387151</v>
+      </c>
+      <c r="V4" s="21"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <f>C3/(C4*Parameters!C7)</f>
         <v>0.4</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="H5" s="24">
+      <c r="G5" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="23">
         <v>1.8288</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="52" t="s">
-        <v>182</v>
-      </c>
-      <c r="K5" s="29" t="s">
+      <c r="I5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" s="21">
+      <c r="M5" s="20">
         <f>Parameters!C3/Parameters!C5</f>
         <v>270</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q5" s="21" t="s">
+      <c r="O5" s="30"/>
+      <c r="P5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="23">
         <v>62.21</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="23">
         <f t="shared" ref="S5:S10" si="1">R5</f>
         <v>62.21</v>
       </c>
-      <c r="T5" s="24">
+      <c r="T5" s="23">
         <f>Parameters!C11</f>
         <v>50</v>
       </c>
-      <c r="U5" s="24">
+      <c r="U5" s="23">
         <f t="shared" si="0"/>
         <v>24.42</v>
       </c>
-      <c r="V5" s="21"/>
+      <c r="V5" s="20"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="C6" s="20">
+        <f>Parameters!C11*C19</f>
+        <v>28.647889789276149</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="21">
-        <f>Parameters!C11*Parameters!C12</f>
-        <v>45</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="24">
+      <c r="E6" s="24"/>
+      <c r="F6" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="23">
         <v>6.5698400000000001</v>
       </c>
-      <c r="I6" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="52"/>
-      <c r="K6" s="29" t="s">
+      <c r="I6" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="59"/>
+      <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="23">
         <f>0.612*Parameters!C6*M5/SQRT(3)</f>
         <v>81.091154708759703</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q6" s="21" t="s">
+      <c r="O6" s="21"/>
+      <c r="P6" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q6" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="23">
         <v>4.75</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="23">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="23">
         <f>Parameters!C13</f>
         <v>4</v>
       </c>
-      <c r="U6" s="24">
+      <c r="U6" s="23">
         <f t="shared" si="0"/>
         <v>18.75</v>
       </c>
-      <c r="V6" s="21"/>
+      <c r="V6" s="20"/>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <f>Parameters!C2/(Parameters!C8*2*Parameters!H8/60)</f>
         <v>127.32395461900511</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="30" t="s">
+      <c r="D7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" s="24">
+      <c r="H7" s="23">
         <f>Parameters!C15*H13*Parameters!H8*(H5/2)^2*1.25</f>
         <v>197.00786764799284</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="29" t="s">
+      <c r="I7" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="M7" s="24">
+      <c r="M7" s="23">
         <f>M4/(Parameters!H3*'General Calculations'!M6*3)</f>
         <v>9.7177314523144265</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q7" s="21" t="s">
+      <c r="O7" s="30"/>
+      <c r="P7" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="23">
         <v>351.3</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="23">
         <f t="shared" si="1"/>
         <v>351.3</v>
       </c>
-      <c r="T7" s="24">
+      <c r="T7" s="23">
         <f>H22</f>
-        <v>178.68046222001527</v>
-      </c>
-      <c r="U7" s="24">
+        <v>75.503284847670415</v>
+      </c>
+      <c r="U7" s="23">
         <f t="shared" si="0"/>
-        <v>96.607953457962566</v>
-      </c>
-      <c r="V7" s="21"/>
+        <v>365.27776997882376</v>
+      </c>
+      <c r="V7" s="20"/>
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="33">
+        <f>C7/(2*C6*1000)</f>
+        <v>2.2222222222222222E-3</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="34">
-        <f>2*C7/(C6*1000*Parameters!H8)</f>
-        <v>1.8012654910913857E-3</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="29" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="21">
+      <c r="L8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="20">
         <f>Parameters!C8*'General Calculations'!C4/120</f>
         <v>100</v>
       </c>
-      <c r="N8" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="O8" s="31"/>
-      <c r="P8" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="R8" s="24">
+      <c r="N8" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="O8" s="30"/>
+      <c r="P8" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="R8" s="23">
         <f>21</f>
         <v>21</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="23">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="T8" s="24">
+      <c r="T8" s="23">
         <f>C7</f>
         <v>127.32395461900511</v>
       </c>
-      <c r="U8" s="24">
+      <c r="U8" s="23">
         <f t="shared" si="0"/>
         <v>83.506638587500007</v>
       </c>
-      <c r="V8" s="21"/>
+      <c r="V8" s="20"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="A9" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="33">
+        <f>4*C8/Parameters!H8</f>
+        <v>2.8294212137556689E-3</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="24">
+      <c r="R9" s="23">
         <f>1.26</f>
         <v>1.26</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="23">
         <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
-      <c r="T9" s="24">
+      <c r="T9" s="23">
         <f>M21</f>
-        <v>0.5195961563928515</v>
-      </c>
-      <c r="U9" s="24">
+        <v>0.75422189569649689</v>
+      </c>
+      <c r="U9" s="23">
         <f t="shared" si="0"/>
-        <v>142.49602012978534</v>
-      </c>
-      <c r="V9" s="21"/>
+        <v>67.059589119517028</v>
+      </c>
+      <c r="V9" s="20"/>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="33">
-        <v>200</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q10" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="R10" s="36">
+      <c r="R10" s="35">
         <v>105.62</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="23">
         <f t="shared" si="1"/>
         <v>105.62</v>
       </c>
-      <c r="T10" s="24">
-        <f>C11+C16</f>
-        <v>184.42661945624999</v>
-      </c>
-      <c r="U10" s="24">
+      <c r="T10" s="23">
+        <f>C12+C17</f>
+        <v>96.555114987268894</v>
+      </c>
+      <c r="U10" s="23">
         <f t="shared" si="0"/>
-        <v>42.730609978428106</v>
+        <v>9.3883011934959075</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="33">
-        <v>150</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="30" t="s">
+      <c r="A11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="32">
+        <f>1000*(C9/C10)^(1/3)</f>
+        <v>211.2801923321104</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="20">
         <v>0.93300000000000005</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="L11" s="21" t="s">
+      <c r="J11" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="K11" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="21">
-        <v>17</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O11" s="52" t="s">
-        <v>182</v>
-      </c>
-      <c r="P11" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q11" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="R11" s="36">
+      <c r="L11" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="M11" s="20">
+        <v>15</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="P11" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="R11" s="35">
         <f>0.6986*1000</f>
         <v>698.6</v>
       </c>
-      <c r="S11" s="36">
+      <c r="S11" s="35">
         <f>R11/4</f>
         <v>174.65</v>
       </c>
-      <c r="T11" s="24">
+      <c r="T11" s="23">
         <f>H19</f>
-        <v>157.67616000000001</v>
-      </c>
-      <c r="U11" s="24">
+        <v>66.627698821977219</v>
+      </c>
+      <c r="U11" s="23">
         <f t="shared" si="0"/>
-        <v>10.765000872674724</v>
+        <v>162.12821857565268</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="24">
-        <v>1.4</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="A12" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="32">
+        <f>C11*C10</f>
+        <v>63.384057699633118</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="37">
+        <f>0.001*2*C11*C12*Parameters!C12/C4</f>
+        <v>1.2052616311411262</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="20">
+        <v>2</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="59"/>
+      <c r="P12" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="38">
-        <f>0.001*2*C10*C11*Parameters!C12/C4</f>
-        <v>2.7</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="M12" s="21">
-        <v>2</v>
-      </c>
-      <c r="N12" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O12" s="52"/>
-      <c r="P12" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12" s="38">
+      <c r="R12" s="37">
         <v>0.93300000000000005</v>
       </c>
-      <c r="S12" s="38">
+      <c r="S12" s="37">
         <f>R12</f>
         <v>0.93300000000000005</v>
       </c>
-      <c r="T12" s="38">
+      <c r="T12" s="37">
         <f>H11</f>
         <v>0.93300000000000005</v>
       </c>
-      <c r="U12" s="24">
+      <c r="U12" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="20">
+        <v>30</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" s="20">
+        <v>2</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" s="59"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="38"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="33">
-        <f>C12*C10</f>
-        <v>280</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="21">
-        <v>30</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="M13" s="21">
-        <v>2</v>
-      </c>
-      <c r="N13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O13" s="52"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-    </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="21">
-        <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="29" t="s">
+      <c r="C14" s="32">
+        <f>C13*C11</f>
+        <v>253.53623079853247</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H14" s="21">
+      <c r="H14" s="20">
         <f>H13*Parameters!C9*Parameters!C15/2</f>
         <v>60</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="30" t="s">
+      <c r="J14" s="21"/>
+      <c r="K14" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="L14" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="M14" s="23">
+        <f>C14/2-C11/2-M11-M12-M13-M19</f>
+        <v>0.12801923321103459</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="20">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="23">
+        <f>4.44*H12*M8*H14*H11/1000</f>
+        <v>29.956922473408429</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="M15" s="22">
+        <v>13</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="O15" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="23">
+        <f>Parameters!H8*C11/'General Calculations'!C3</f>
+        <v>27.65651247171435</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="H16" s="20">
+        <f>H15*Parameters!C4</f>
+        <v>119.82768989363372</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="M16" s="23">
+        <f>C17-M15</f>
+        <v>20.171057287635783</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="38"/>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="23">
+        <f>Parameters!H8*(C14-M14)/'General Calculations'!C3</f>
+        <v>33.171057287635783</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="M17" s="23">
+        <f>C16-M15</f>
+        <v>14.65651247171435</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="21"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" s="37">
+        <f>(M15)/C16</f>
+        <v>0.47005203614503915</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="23">
+        <f>2*Parameters!C9*C12*1.2</f>
+        <v>304.24347695823894</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="40"/>
+      <c r="K18" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="M14" s="24">
-        <f>C13/2-C10/2-M11-M12-M13-M19</f>
-        <v>17</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-    </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="24">
-        <f>Parameters!H8*C10/'General Calculations'!C3</f>
-        <v>26.179938750000002</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="24">
-        <f>4.44*H12*M8*H14*H11/1000</f>
-        <v>67.108824000000027</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="M15" s="23">
-        <v>8</v>
-      </c>
-      <c r="N15" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="O15" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="39"/>
-    </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="24">
-        <f>Parameters!H8*(C13-M14)/'General Calculations'!C3</f>
-        <v>34.426619456250002</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="M16" s="24">
-        <f>C16-M15</f>
-        <v>26.426619456250002</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O16" s="22"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="39"/>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="L17" s="21" t="s">
+      <c r="L18" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="M17" s="24">
-        <f>C15-M15</f>
-        <v>18.179938750000002</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O17" s="22"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="H18" s="24">
-        <f>2*Parameters!C9*C11*1.2</f>
-        <v>720</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="M18" s="21">
+      <c r="M18" s="20">
         <v>2.5</v>
       </c>
-      <c r="N18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O18" s="21"/>
-      <c r="R18" s="39">
+      <c r="N18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="R18" s="38">
         <f>80*4*SQRT(3)</f>
         <v>554.25625842204067</v>
       </c>
-      <c r="S18" s="39"/>
-      <c r="T18" s="39"/>
-      <c r="U18" s="39"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
     </row>
     <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="29" t="s">
+      <c r="A19" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="37">
+        <f>Parameters!C12*2/Parameters!H8</f>
+        <v>0.57295779578552297</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="23">
+        <f>H18*H6/(H13)</f>
+        <v>66.627698821977219</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="M19" s="20">
+        <v>2</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63">
+        <f>C19*PI()/2/C18</f>
+        <v>1.91468163484499</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="20">
+        <f>M7^2*H19/1000</f>
+        <v>6.2919404039725348</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="K20" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="M20" s="23">
+        <f>(M16+M17)*M11/2</f>
+        <v>261.206773195126</v>
+      </c>
+      <c r="N20" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="20"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="20">
+        <v>0</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M21" s="23">
+        <f>H7/M20</f>
+        <v>0.75422189569649689</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="20"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G22" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H22" s="20">
+        <f>H20*Parameters!C4*Parameters!C7+H21</f>
+        <v>75.503284847670415</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="H19" s="24">
-        <f>H18*H6/(H13)</f>
-        <v>157.67616000000001</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="M19" s="21">
-        <v>2</v>
-      </c>
-      <c r="N19" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O19" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="33">
-        <f>1000*(C8/C9)^(1/3)</f>
-        <v>153.29779501892307</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="H20" s="21">
-        <f>M7^2*H19/1000</f>
-        <v>14.890038518334606</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="24">
-        <f>(M16+M17)*M11/2</f>
-        <v>379.15574475312502</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="O20" s="21"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-    </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="33">
-        <f>C10*C9</f>
-        <v>100</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="G21" s="21" t="s">
+      <c r="G23" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="20">
+        <f>Parameters!C2/(Parameters!C2+'General Calculations'!H22)*100</f>
+        <v>99.065033073674314</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="46"/>
+      <c r="K23" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="H21" s="21">
-        <v>0</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="M21" s="24">
-        <f>H7/M20</f>
-        <v>0.5195961563928515</v>
-      </c>
-      <c r="N21" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="O21" s="21"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="H22" s="21">
-        <f>H20*Parameters!C4*Parameters!C7+H21</f>
-        <v>178.68046222001527</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="H23" s="21">
-        <f>Parameters!C2/(Parameters!C2+'General Calculations'!H22)*100</f>
-        <v>97.815289849684206</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="M24" s="38">
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="M24" s="37">
         <f>2*Parameters!H8*Parameters!C16/'General Calculations'!C4</f>
         <v>0.2199114855</v>
       </c>
-      <c r="N24" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="O24" s="21"/>
+      <c r="N24" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="O24" s="20"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="L25" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="M25" s="21">
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="M25" s="20">
         <f>M24*180/Parameters!H8</f>
         <v>12.6</v>
       </c>
-      <c r="N25" s="21" t="s">
+      <c r="N25" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="M26" s="23">
+        <f>(M24*(C11/2-C15/2)+2*C15)*(C12+2*C15)/100</f>
+        <v>16.425465688366973</v>
+      </c>
+      <c r="N26" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26" s="26"/>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="28"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="M27" s="23">
+        <f>(M24*(C11/2-C15/2-Parameters!C14/2)+2*C15)*(C12)/100</f>
+        <v>15.679104953696651</v>
+      </c>
+      <c r="N27" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="M28" s="23">
+        <f>M27/M26</f>
+        <v>0.95456075652096017</v>
+      </c>
+      <c r="N28" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="H29" s="20">
+        <v>1.05</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="K29" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="M26" s="24">
-        <f>(M24*(C10/2-C14/2)+2*C14)*(C11+2*C14)/100</f>
-        <v>34.965264757777192</v>
-      </c>
-      <c r="N26" s="21" t="s">
+      <c r="L29" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="O26" s="27"/>
-    </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="29"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="30" t="s">
+      <c r="M29" s="23">
+        <f>M27*C15/(M26*Parameters!C14)</f>
+        <v>0.27273164472027434</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O29" s="20"/>
+      <c r="P29" s="25">
+        <f>1/M29</f>
+        <v>3.6666078885918951</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="H30" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="M30" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="58" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="H31" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="I31" s="40"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="L27" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="M27" s="24">
-        <f>(M24*(C10/2-C14/2-Parameters!C14/2)+2*C14)*(C11)/100</f>
-        <v>34.110495007087501</v>
-      </c>
-      <c r="N27" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="O27" s="21"/>
-    </row>
-    <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="30" t="s">
+      <c r="L31" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="M31" s="47">
+        <f>M30*Parameters!H11</f>
+        <v>1.3823007660000001E-6</v>
+      </c>
+      <c r="N31" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="F32" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="H32" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I32" s="20"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="L28" s="21" t="s">
+      <c r="L32" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="M28" s="24">
-        <f>M27/M26</f>
-        <v>0.97555374579282805</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O28" s="21"/>
-    </row>
-    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H29" s="21">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" s="45"/>
-      <c r="K29" s="30" t="s">
+      <c r="M32" s="23">
+        <v>1</v>
+      </c>
+      <c r="N32" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O32" s="58" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="6:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="F33" s="29"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L33" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="L29" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="M29" s="24">
-        <f>M27*C14/(M26*Parameters!C14)</f>
-        <v>0.16723778499305625</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O29" s="21"/>
-    </row>
-    <row r="30" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="H30" s="21">
-        <v>0.15</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="45"/>
-      <c r="K30" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="L30" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="M30" s="21">
-        <v>1000</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O30" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="30"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="L31" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="M31" s="49">
-        <f>M30*Parameters!H11</f>
-        <v>1.2566370599999999E-3</v>
-      </c>
-      <c r="N31" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="O31" s="21"/>
-    </row>
-    <row r="32" spans="1:21" ht="18" x14ac:dyDescent="0.25">
-      <c r="F32" s="30"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="L32" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M32" s="24">
-        <v>1</v>
-      </c>
-      <c r="N32" s="21" t="s">
+      <c r="M33" s="23">
+        <f>M28*M32/(1+M30*M29*H29*(1+H30))</f>
+        <v>0.70072063671599039</v>
+      </c>
+      <c r="N33" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O32" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="6:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="F33" s="30"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="M33" s="24">
-        <f>M28/(1+M30*M29*H29*(1+H30))</f>
-        <v>4.5896360150966195E-3</v>
-      </c>
-      <c r="N33" s="21" t="s">
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="6:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="K34" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="M34" s="23">
+        <f>M28*M32*H31/(1+H32*M30*M29)</f>
+        <v>0.6818263998174523</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O33" s="21"/>
-    </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4159,12 +4663,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="103" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Visio.Drawing.15" shapeId="5121" r:id="rId3">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>6848475</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>352425</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Visio.Drawing.15" shapeId="5121" r:id="rId3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4252,7 +4812,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="12">
         <v>2</v>
@@ -4302,7 +4862,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" s="14">
         <v>2</v>
@@ -4339,10 +4899,10 @@
         <v>127.32395461900511</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="14">
         <f>2-((H5)/2-1)*0.1</f>
@@ -4385,15 +4945,15 @@
         <v>1.01</v>
       </c>
       <c r="R7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C8" s="8">
         <f>Parameters!C2/(Parameters!C4*Parameters!H2/100)</f>
@@ -4405,10 +4965,10 @@
     </row>
     <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="C9" s="7">
         <f>Parameters!C3/Parameters!C5</f>
@@ -4435,13 +4995,13 @@
     </row>
     <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="C11" s="8">
-        <f>C8/(Parameters!H3*'Calculations-old'!C10*3)</f>
+        <f>C8/(Parameters!H3*'Not used-old'!C10*3)</f>
         <v>9.7177314523144265</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -4453,44 +5013,44 @@
         <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="7">
+        <f>Parameters!C8*'Not used-old'!C4/120</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="C12" s="7">
-        <f>Parameters!C8*'Calculations-old'!C4/120</f>
-        <v>100</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="C13" s="7">
         <f>Parameters!C11*Parameters!C12</f>
         <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="9">
         <f>2*C7/(C13*1000*Parameters!H8)</f>
         <v>1.8012654910913857E-3</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14">
         <f>0.155^2*150</f>
@@ -4502,10 +5062,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="C15" s="7">
         <v>0.3</v>
@@ -4514,7 +5074,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K15">
         <v>150</v>
@@ -4522,41 +5082,41 @@
     </row>
     <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="C16" s="10">
         <f>1000*(C14/C15)^(1/3)</f>
         <v>181.7546335652992</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="C17" s="10">
         <f>C16*C15</f>
         <v>54.526390069589759</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="8">
         <v>1.4</v>
@@ -4565,76 +5125,76 @@
         <v>15</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="C19" s="10">
         <f>C18*C16</f>
         <v>254.45648699141887</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="C20" s="7">
         <f>ROUND(((0.18+0.006*(Parameters!C2)^0.4)*1.6),1)</f>
         <v>0.6</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="8">
-        <f>Parameters!H8*'Calculations-old'!C16/'Calculations-old'!C3</f>
+        <f>Parameters!H8*'Not used-old'!C16/'Not used-old'!C3</f>
         <v>23.791625871341139</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="15">
+        <f>0.001*2*C16*C17*Parameters!C12/'Not used-old'!C4</f>
+        <v>0.891938164206317</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C22" s="15">
-        <f>0.001*2*C16*C17*Parameters!C12/'Calculations-old'!C4</f>
-        <v>0.891938164206317</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="7">
         <v>100</v>
@@ -4645,10 +5205,10 @@
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="C24" s="7">
         <f>C23*Parameters!C9*Parameters!C15/2</f>
@@ -4660,10 +5220,10 @@
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="C25" s="8">
         <f>4.44*C24*C12*C22*C6/1000</f>
@@ -4698,208 +5258,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L18"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="12">
-        <v>2</v>
-      </c>
-      <c r="C1" s="12">
-        <v>4</v>
-      </c>
-      <c r="D1" s="12">
-        <v>6</v>
-      </c>
-      <c r="E1" s="12">
-        <v>8</v>
-      </c>
-      <c r="F1" s="12">
-        <v>10</v>
-      </c>
-      <c r="G1" s="12">
-        <v>12</v>
-      </c>
-      <c r="H1" s="12">
-        <v>14</v>
-      </c>
-      <c r="I1" s="12">
-        <v>16</v>
-      </c>
-      <c r="J1" s="12">
-        <v>18</v>
-      </c>
-      <c r="K1" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="14">
-        <v>2</v>
-      </c>
-      <c r="C2" s="14">
-        <v>1.88</v>
-      </c>
-      <c r="D2" s="14">
-        <v>1.78</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1.66</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1.54</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1.43</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="14">
-        <f>2-((B1)/2-1)*0.1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="14">
-        <f>2-((C1)/2-1)*0.115</f>
-        <v>1.885</v>
-      </c>
-      <c r="D3" s="14">
-        <f>2-((D1)/2-1)*0.115</f>
-        <v>1.77</v>
-      </c>
-      <c r="E3" s="14">
-        <f>2-((E1)/2-1)*0.115</f>
-        <v>1.655</v>
-      </c>
-      <c r="F3" s="14">
-        <f>2-((F1)/2-1)*0.115</f>
-        <v>1.54</v>
-      </c>
-      <c r="G3" s="14">
-        <f>2-((G1)/2-1)*0.115</f>
-        <v>1.4249999999999998</v>
-      </c>
-      <c r="H3" s="14">
-        <f>2-((H1)/2-1)*0.11</f>
-        <v>1.3399999999999999</v>
-      </c>
-      <c r="I3" s="14">
-        <f>2-((I1)/2-1)*0.11</f>
-        <v>1.23</v>
-      </c>
-      <c r="J3" s="14">
-        <f>2-((J1)/2-1)*0.11</f>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="K3" s="14">
-        <f>2-((K1)/2-1)*0.11</f>
-        <v>1.01</v>
-      </c>
-      <c r="L3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>